<commit_message>
option to calculate simple rate instead of compound
</commit_message>
<xml_diff>
--- a/ZopaTest.Tests/compounded_loan_rate.xlsx
+++ b/ZopaTest.Tests/compounded_loan_rate.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafal\Documents\pracuj\UK\autumn 2017\Zopa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafal\Documents\github\ZopaTest\ZopaTest.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{1C590916-E2A3-4457-A543-2F1AE2FC7441}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="2" xr2:uid="{1C590916-E2A3-4457-A543-2F1AE2FC7441}"/>
   </bookViews>
   <sheets>
     <sheet name="compound rate" sheetId="1" r:id="rId1"/>
     <sheet name="lenders spread" sheetId="2" r:id="rId2"/>
+    <sheet name="simple rateloa" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -73,6 +74,18 @@
   </si>
   <si>
     <t>as fraction</t>
+  </si>
+  <si>
+    <t>loan amount</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>simple interest</t>
+  </si>
+  <si>
+    <t>monthly repayment</t>
   </si>
 </sst>
 </file>
@@ -437,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185077D2-D769-434F-89C3-770770282070}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -642,7 +655,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,4 +759,114 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F4BF7B-15C7-408B-8A45-0ABCB304D6FB}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>18000</v>
+      </c>
+      <c r="B2">
+        <v>0.06</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <f>$A2*$B2*$C2</f>
+        <v>3240</v>
+      </c>
+      <c r="E2">
+        <f>$A2+$D2</f>
+        <v>21240</v>
+      </c>
+      <c r="F2">
+        <f>$E2/($C2*12)</f>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1100</v>
+      </c>
+      <c r="B3">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <f>$A3*$B3*$C3</f>
+        <v>227.70000000000002</v>
+      </c>
+      <c r="E3">
+        <f>$A3+$D3</f>
+        <v>1327.7</v>
+      </c>
+      <c r="F3">
+        <f>$E3/($C3*12)</f>
+        <v>36.88055555555556</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f>$A4*$B4*$C4</f>
+        <v>210</v>
+      </c>
+      <c r="E4">
+        <f>$A4+$D4</f>
+        <v>1210</v>
+      </c>
+      <c r="F4">
+        <f>$E4/($C4*12)</f>
+        <v>33.611111111111114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>